<commit_message>
Add Excel parsing CLI tool and update specifications handling
</commit_message>
<xml_diff>
--- a/packages/events/src/examples/specifications.xlsx
+++ b/packages/events/src/examples/specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.houston/nhs-notify/nhs-notify-supplier-config/packages/events/src/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31FE2C9-4144-9C44-A9C7-5EB8BFD39FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BEB526-4605-FC4E-AC22-B322DC898EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" activeTab="1" xr2:uid="{7C1C9A7A-5291-284B-B7CE-72455DFF925E}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" xr2:uid="{7C1C9A7A-5291-284B-B7CE-72455DFF925E}"/>
   </bookViews>
   <sheets>
     <sheet name="PackSpecification" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>PUBLISHED</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
   </si>
   <si>
     <t>2023-01-01T00:00:00.000Z</t>
@@ -536,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F391B7A5-CD97-A14C-80A9-E44FAC84811F}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,135 +584,135 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>29</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -728,7 +725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D549C18-D7B6-3340-906F-031EB109A9B7}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -754,36 +751,36 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -791,19 +788,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -811,19 +808,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -831,19 +828,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -851,28 +848,28 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance PackSpecification and Excel parsing to support optional billingId and detailed postage attributes
</commit_message>
<xml_diff>
--- a/packages/events/src/examples/specifications.xlsx
+++ b/packages/events/src/examples/specifications.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.houston/nhs-notify/nhs-notify-supplier-config/packages/events/src/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BEB526-4605-FC4E-AC22-B322DC898EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89186C5-4D98-924C-8414-6B472FBC3AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" xr2:uid="{7C1C9A7A-5291-284B-B7CE-72455DFF925E}"/>
+    <workbookView xWindow="-7580" yWindow="-26580" windowWidth="34560" windowHeight="21660" activeTab="1" xr2:uid="{7C1C9A7A-5291-284B-B7CE-72455DFF925E}"/>
   </bookViews>
   <sheets>
-    <sheet name="PackSpecification" sheetId="1" r:id="rId1"/>
-    <sheet name="LetterVariant" sheetId="2" r:id="rId2"/>
+    <sheet name="LetterVariant" sheetId="2" r:id="rId1"/>
+    <sheet name="PackSpecification" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -160,6 +160,36 @@
   </si>
   <si>
     <t>Client 1 Letter Variant 1</t>
+  </si>
+  <si>
+    <t>billingId</t>
+  </si>
+  <si>
+    <t>admail-insert</t>
+  </si>
+  <si>
+    <t>postage.tariff</t>
+  </si>
+  <si>
+    <t>postage.maxSheets</t>
+  </si>
+  <si>
+    <t>economy</t>
+  </si>
+  <si>
+    <t>articles-blind</t>
+  </si>
+  <si>
+    <t>firstclass</t>
+  </si>
+  <si>
+    <t>admail</t>
+  </si>
+  <si>
+    <t>postage.size</t>
+  </si>
+  <si>
+    <t>LARGE</t>
   </si>
 </sst>
 </file>
@@ -530,198 +560,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F391B7A5-CD97-A14C-80A9-E44FAC84811F}">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D549C18-D7B6-3340-906F-031EB109A9B7}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -878,6 +716,270 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F391B7A5-CD97-A14C-80A9-E44FAC84811F}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{6be7ebee-5b98-4973-86ef-ae3752ea54e7}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="0" removed="0"/>

</xml_diff>